<commit_message>
Changed some data sets in the excel files
</commit_message>
<xml_diff>
--- a/data/CreateLead.xlsx
+++ b/data/CreateLead.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Company</t>
   </si>
@@ -64,6 +64,21 @@
   </si>
   <si>
     <t>amitkumar@gmail.com</t>
+  </si>
+  <si>
+    <t>FIS</t>
+  </si>
+  <si>
+    <t>Vibhuti</t>
+  </si>
+  <si>
+    <t>Mishra</t>
+  </si>
+  <si>
+    <t>8979466578</t>
+  </si>
+  <si>
+    <t>vibhuti.mishra@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -393,11 +408,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -456,10 +469,28 @@
         <v>14</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
     <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>